<commit_message>
updation of custom order
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageClaims.xlsx
+++ b/testdata/FCfiles/qa/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="206">
   <si>
     <t>shipmentType</t>
   </si>
@@ -608,6 +608,45 @@
   </si>
   <si>
     <t>DropOff445</t>
+  </si>
+  <si>
+    <t>58532881</t>
+  </si>
+  <si>
+    <t>01-03-2022</t>
+  </si>
+  <si>
+    <t>$746.07</t>
+  </si>
+  <si>
+    <t>FCT927602323742523392</t>
+  </si>
+  <si>
+    <t>FCTEST1004149</t>
+  </si>
+  <si>
+    <t>PickUp791</t>
+  </si>
+  <si>
+    <t>DropOff174</t>
+  </si>
+  <si>
+    <t>58532883</t>
+  </si>
+  <si>
+    <t>$724.75</t>
+  </si>
+  <si>
+    <t>FCT927613389826424832</t>
+  </si>
+  <si>
+    <t>FCTEST1004151</t>
+  </si>
+  <si>
+    <t>PickUp469</t>
+  </si>
+  <si>
+    <t>DropOff759</t>
   </si>
 </sst>
 </file>
@@ -636,7 +675,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="232">
+  <fills count="298">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1793,8 +1832,338 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="230">
+  <borders count="296">
     <border>
       <left/>
       <right/>
@@ -2840,11 +3209,242 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="174">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -2985,7 +3585,40 @@
     <xf applyBorder="true" applyFill="true" borderId="223" fillId="225" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="225" fillId="227" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="227" fillId="229" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="231" borderId="229" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="229" fillId="231" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="231" fillId="233" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="233" fillId="235" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="235" fillId="237" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="237" fillId="239" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="239" fillId="241" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="241" fillId="243" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="243" fillId="245" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="245" fillId="247" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="247" fillId="249" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="249" fillId="251" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="251" fillId="253" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="253" fillId="255" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="255" fillId="257" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="257" fillId="259" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="259" fillId="261" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="261" fillId="263" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="263" fillId="265" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="265" fillId="267" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="267" fillId="269" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="269" fillId="271" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="271" fillId="273" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="273" fillId="275" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="275" fillId="277" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="277" fillId="279" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="279" fillId="281" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="281" fillId="283" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="283" fillId="285" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="285" fillId="287" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="287" fillId="289" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="289" fillId="291" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="291" fillId="293" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="293" fillId="295" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="297" borderId="295" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -3446,8 +4079,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="133" t="s">
-        <v>191</v>
+      <c r="C2" s="166" t="s">
+        <v>204</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -3470,8 +4103,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="134" t="s">
-        <v>192</v>
+      <c r="K2" s="167" t="s">
+        <v>205</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -3616,8 +4249,8 @@
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="111" t="s">
-        <v>178</v>
+      <c r="B2" s="143" t="s">
+        <v>194</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -3668,22 +4301,22 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="110" t="s">
-        <v>183</v>
-      </c>
-      <c r="U2" s="112" t="s">
-        <v>145</v>
+      <c r="T2" s="142" t="s">
+        <v>193</v>
+      </c>
+      <c r="U2" s="144" t="s">
+        <v>195</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="113" t="s">
-        <v>184</v>
-      </c>
-      <c r="X2" s="114" t="s">
-        <v>185</v>
-      </c>
-      <c r="Y2" s="115" t="s">
+      <c r="W2" s="145" t="s">
+        <v>196</v>
+      </c>
+      <c r="X2" s="146" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y2" s="147" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3691,8 +4324,8 @@
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="127" t="s">
-        <v>178</v>
+      <c r="B3" s="160" t="s">
+        <v>194</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -3743,22 +4376,22 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="126" t="s">
-        <v>188</v>
-      </c>
-      <c r="U3" s="128" t="s">
-        <v>161</v>
+      <c r="T3" s="159" t="s">
+        <v>200</v>
+      </c>
+      <c r="U3" s="161" t="s">
+        <v>201</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W3" s="129" t="s">
-        <v>189</v>
-      </c>
-      <c r="X3" s="130" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y3" s="131"/>
+      <c r="W3" s="162" t="s">
+        <v>202</v>
+      </c>
+      <c r="X3" s="163" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y3" s="164"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -3916,7 +4549,7 @@
       <c r="B2" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="124" t="s">
+      <c r="C2" s="156" t="s">
         <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3960,7 +4593,7 @@
       <c r="B3" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="140" t="s">
+      <c r="C3" s="173" t="s">
         <v>137</v>
       </c>
       <c r="D3" s="15" t="s">

</xml_diff>